<commit_message>
very large and late update
</commit_message>
<xml_diff>
--- a/assemblynode_commitment.xlsx
+++ b/assemblynode_commitment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SusanaLopezLemarroy/Documents/Vrije_University_in_Amsterdam/INTERNSHIPs/Minor/tomato-rhizosphere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85156D1E-8F84-4B46-B012-B8BCCBBAB1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC41A53E-D235-4145-BDD9-7E35F51E1C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="17100" windowHeight="17620" xr2:uid="{7CDAEA52-EF8C-F547-9DD4-5CF0429F0995}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="86">
   <si>
     <t>sample</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>19.10.2022</t>
+  </si>
+  <si>
+    <t>21.10.2022</t>
+  </si>
+  <si>
+    <t>23.10.2022</t>
+  </si>
+  <si>
+    <t>24.10.2022</t>
   </si>
 </sst>
 </file>
@@ -855,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED8C9B1-2E7A-3644-8453-742039F44AAA}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1306,6 +1315,15 @@
       <c r="C20" s="15" t="s">
         <v>75</v>
       </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
@@ -1317,6 +1335,15 @@
       <c r="C21" s="15" t="s">
         <v>75</v>
       </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
@@ -1328,6 +1355,15 @@
       <c r="C22" s="15" t="s">
         <v>75</v>
       </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
@@ -1463,6 +1499,15 @@
       <c r="C28" s="16" t="s">
         <v>76</v>
       </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
@@ -1517,8 +1562,15 @@
       <c r="C31" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="2"/>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
@@ -1530,8 +1582,15 @@
       <c r="C32" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
+      <c r="D32">
+        <v>6</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
@@ -1543,8 +1602,15 @@
       <c r="C33" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33" s="3">
+        <v>2</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
@@ -1556,8 +1622,15 @@
       <c r="C34" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="6"/>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
@@ -1569,6 +1642,15 @@
       <c r="C35" s="17" t="s">
         <v>80</v>
       </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
@@ -1580,6 +1662,15 @@
       <c r="C36" s="17" t="s">
         <v>80</v>
       </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
@@ -1591,6 +1682,15 @@
       <c r="C37" s="17" t="s">
         <v>80</v>
       </c>
+      <c r="D37">
+        <v>6</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
@@ -1602,6 +1702,15 @@
       <c r="C38" s="17" t="s">
         <v>81</v>
       </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
@@ -1613,6 +1722,15 @@
       <c r="C39" s="17" t="s">
         <v>81</v>
       </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
@@ -1624,6 +1742,15 @@
       <c r="C40" s="17" t="s">
         <v>81</v>
       </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
@@ -1635,6 +1762,15 @@
       <c r="C41" s="17" t="s">
         <v>81</v>
       </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
@@ -1646,6 +1782,15 @@
       <c r="C42" s="17" t="s">
         <v>82</v>
       </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
@@ -1657,6 +1802,15 @@
       <c r="C43" s="17" t="s">
         <v>82</v>
       </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="26" t="s">
@@ -1668,6 +1822,15 @@
       <c r="C44" s="18" t="s">
         <v>82</v>
       </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="26" t="s">
@@ -1679,6 +1842,15 @@
       <c r="C45" s="18" t="s">
         <v>82</v>
       </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="26" t="s">
@@ -1690,69 +1862,195 @@
       <c r="C46" s="18" t="s">
         <v>82</v>
       </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
+      <c r="B47" s="18">
+        <v>1</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B48" s="18">
+        <v>2</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48">
+        <v>6</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="18">
+        <v>3</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49">
+        <v>6</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="18">
+        <v>4</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50">
+        <v>6</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="18">
+        <v>5</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="19">
+        <v>2</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="19">
+        <v>4</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="19">
+        <v>3</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54">
+        <v>6</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
+      <c r="B55" s="19">
+        <v>5</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
many docs to be deleter from repository later
</commit_message>
<xml_diff>
--- a/assemblynode_commitment.xlsx
+++ b/assemblynode_commitment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SusanaLopezLemarroy/Documents/Vrije_University_in_Amsterdam/INTERNSHIPs/Minor/tomato-rhizosphere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC41A53E-D235-4145-BDD9-7E35F51E1C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD815A3-2965-D146-949B-BD0E58DF5446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17100" windowHeight="17620" xr2:uid="{7CDAEA52-EF8C-F547-9DD4-5CF0429F0995}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28000" windowHeight="18360" xr2:uid="{7CDAEA52-EF8C-F547-9DD4-5CF0429F0995}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="85">
   <si>
     <t>sample</t>
   </si>
@@ -235,9 +235,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>ERROR: Preprocessing/mg.se.fq is empty.</t>
-  </si>
-  <si>
     <t xml:space="preserve">yes </t>
   </si>
   <si>
@@ -259,21 +256,12 @@
     <t>3.10.2022</t>
   </si>
   <si>
-    <t xml:space="preserve">empty but i thought it wasn't </t>
-  </si>
-  <si>
     <t>6.10.2022</t>
   </si>
   <si>
     <t>7.10.2022</t>
   </si>
   <si>
-    <t> T_712_2_125282342.stderr </t>
-  </si>
-  <si>
-    <t xml:space="preserve">reran accidentally </t>
-  </si>
-  <si>
     <t>8.10.2022</t>
   </si>
   <si>
@@ -293,6 +281,15 @@
   </si>
   <si>
     <t>24.10.2022</t>
+  </si>
+  <si>
+    <t>antiSMASH</t>
+  </si>
+  <si>
+    <t>trial</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -378,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -509,11 +506,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -535,13 +556,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,7 +591,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -854,7 +879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -862,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED8C9B1-2E7A-3644-8453-742039F44AAA}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,7 +903,7 @@
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -897,12 +922,14 @@
       <c r="F1" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H1" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -924,14 +951,11 @@
       <c r="G2" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -953,8 +977,11 @@
       <c r="G3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H3" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -976,8 +1003,11 @@
       <c r="G4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -985,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -999,8 +1029,11 @@
       <c r="G5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H5" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -1022,16 +1055,19 @@
       <c r="G6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="H6" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="8">
         <v>2</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -1042,9 +1078,12 @@
       <c r="F7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G7" s="28"/>
+      <c r="H7" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1052,7 +1091,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -1063,9 +1102,12 @@
       <c r="F8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G8" s="29"/>
+      <c r="H8" s="30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1115,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -1082,11 +1124,14 @@
         <v>3</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1094,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1105,9 +1150,12 @@
       <c r="F10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G10" s="7"/>
+      <c r="H10" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
@@ -1115,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -1126,8 +1174,11 @@
       <c r="F11" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1135,7 +1186,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -1146,9 +1197,12 @@
       <c r="F12" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="H12" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="15">
@@ -1169,11 +1223,11 @@
       <c r="G13" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
@@ -1195,8 +1249,11 @@
       <c r="G14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>16</v>
       </c>
@@ -1218,8 +1275,11 @@
       <c r="G15" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
@@ -1240,6 +1300,9 @@
       </c>
       <c r="G16" t="s">
         <v>64</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1259,10 +1322,13 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
         <v>64</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1273,7 +1339,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18">
         <v>8</v>
@@ -1283,6 +1349,9 @@
       </c>
       <c r="F18" t="s">
         <v>62</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1293,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19">
         <v>8</v>
@@ -1302,7 +1371,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1313,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D20">
         <v>8</v>
@@ -1323,6 +1395,9 @@
       </c>
       <c r="F20" t="s">
         <v>62</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1333,7 +1408,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D21">
         <v>8</v>
@@ -1343,6 +1418,9 @@
       </c>
       <c r="F21" t="s">
         <v>62</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1353,7 +1431,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22">
         <v>8</v>
@@ -1363,6 +1441,9 @@
       </c>
       <c r="F22" t="s">
         <v>62</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1373,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23">
         <v>8</v>
@@ -1387,16 +1468,19 @@
       <c r="G23" t="s">
         <v>64</v>
       </c>
+      <c r="H23" s="30" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="16">
         <v>4</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1410,19 +1494,19 @@
       <c r="G24" t="s">
         <v>65</v>
       </c>
-      <c r="H24" t="s">
-        <v>66</v>
+      <c r="H24" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="16">
         <v>5</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25">
         <v>6</v>
@@ -1436,19 +1520,19 @@
       <c r="G25" t="s">
         <v>65</v>
       </c>
-      <c r="H25" t="s">
-        <v>66</v>
+      <c r="H25" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="16">
         <v>2</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -1462,51 +1546,54 @@
       <c r="G26" t="s">
         <v>65</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="16">
+        <v>3</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="16">
+        <v>3</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="16">
-        <v>3</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27">
-        <v>6</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="16">
-        <v>3</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28">
-        <v>6</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28" t="s">
-        <v>67</v>
+      <c r="H28" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1517,7 +1604,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29">
         <v>8</v>
@@ -1531,16 +1618,19 @@
       <c r="G29" t="s">
         <v>64</v>
       </c>
+      <c r="H29" s="30" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="16">
         <v>2</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D30">
         <v>6</v>
@@ -1551,16 +1641,19 @@
       <c r="F30" t="s">
         <v>62</v>
       </c>
+      <c r="H30" s="30" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="16">
         <v>3</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D31">
         <v>6</v>
@@ -1571,16 +1664,19 @@
       <c r="F31" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="H31" s="30" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="22" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="16">
         <v>4</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -1591,16 +1687,19 @@
       <c r="F32" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+      <c r="H32" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="22" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="16">
         <v>5</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>6</v>
@@ -1609,18 +1708,21 @@
         <v>2</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="24" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="17">
         <v>3</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D34">
         <v>7</v>
@@ -1631,16 +1733,19 @@
       <c r="F34" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="25" t="s">
+      <c r="H34" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D35">
         <v>6</v>
@@ -1651,16 +1756,19 @@
       <c r="F35" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="25" t="s">
+      <c r="H35" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="17">
         <v>4</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -1671,16 +1779,19 @@
       <c r="F36" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="25" t="s">
+      <c r="H36" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="24" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="17">
         <v>5</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D37">
         <v>6</v>
@@ -1691,16 +1802,19 @@
       <c r="F37" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="25" t="s">
+      <c r="H37" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="24" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="17">
         <v>1</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D38">
         <v>6</v>
@@ -1711,16 +1825,19 @@
       <c r="F38" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="25" t="s">
+      <c r="H38" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="24" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="17">
         <v>3</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D39">
         <v>6</v>
@@ -1731,16 +1848,19 @@
       <c r="F39" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="25" t="s">
+      <c r="H39" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="17">
         <v>4</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D40">
         <v>6</v>
@@ -1751,16 +1871,19 @@
       <c r="F40" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="25" t="s">
+      <c r="H40" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="17">
         <v>5</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D41">
         <v>6</v>
@@ -1771,16 +1894,19 @@
       <c r="F41" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
+      <c r="H41" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="24" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="17">
         <v>1</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D42">
         <v>6</v>
@@ -1791,16 +1917,19 @@
       <c r="F42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="H42" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="17">
         <v>2</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D43">
         <v>6</v>
@@ -1809,18 +1938,21 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="18">
         <v>3</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D44">
         <v>6</v>
@@ -1831,16 +1963,19 @@
       <c r="F44" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="26" t="s">
+      <c r="H44" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="18">
         <v>4</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D45">
         <v>6</v>
@@ -1851,16 +1986,19 @@
       <c r="F45" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="26" t="s">
+      <c r="H45" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="18">
         <v>5</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -1871,16 +2009,19 @@
       <c r="F46" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="26" t="s">
+      <c r="H46" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="25" t="s">
         <v>48</v>
       </c>
       <c r="B47" s="18">
         <v>1</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D47">
         <v>6</v>
@@ -1891,16 +2032,19 @@
       <c r="F47" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="26" t="s">
+      <c r="H47" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="18">
         <v>2</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D48">
         <v>6</v>
@@ -1911,16 +2055,19 @@
       <c r="F48" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="26" t="s">
+      <c r="H48" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B49" s="18">
         <v>3</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D49">
         <v>6</v>
@@ -1931,16 +2078,19 @@
       <c r="F49" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="26" t="s">
+      <c r="H49" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="25" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="18">
         <v>4</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D50">
         <v>6</v>
@@ -1951,16 +2101,19 @@
       <c r="F50" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="26" t="s">
+      <c r="H50" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="18">
         <v>5</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D51">
         <v>6</v>
@@ -1971,16 +2124,19 @@
       <c r="F51" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="27" t="s">
+      <c r="H51" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="26" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="19">
         <v>2</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D52">
         <v>6</v>
@@ -1991,16 +2147,19 @@
       <c r="F52" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="27" t="s">
+      <c r="H52" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="26" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="19">
         <v>4</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D53">
         <v>6</v>
@@ -2011,16 +2170,19 @@
       <c r="F53" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="27" t="s">
+      <c r="H53" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="19">
         <v>3</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D54">
         <v>6</v>
@@ -2031,16 +2193,19 @@
       <c r="F54" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="27" t="s">
+      <c r="H54" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="19">
         <v>5</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D55">
         <v>6</v>
@@ -2050,6 +2215,9 @@
       </c>
       <c r="F55" t="s">
         <v>62</v>
+      </c>
+      <c r="H55" s="30" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>